<commit_message>
[DrSpot] Add all illumination sources and 100% SpO2 PPG spectrum
</commit_message>
<xml_diff>
--- a/vitals_collection/drspot/docs/pulse_signature_vector.xlsx
+++ b/vitals_collection/drspot/docs/pulse_signature_vector.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t xml:space="preserve">Illumination</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">Sunlight</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluorescent</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cool white LED</t>
   </si>
   <si>
@@ -128,9 +125,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -208,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +239,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -258,12 +260,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:AMJ71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="10" topLeftCell="B11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="T71" activeCellId="0" sqref="T71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -306,7 +308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -330,7 +332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
@@ -350,7 +352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
@@ -408,13 +410,12 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="T9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="5" t="s">
@@ -456,7 +457,7 @@
       <c r="Q10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -468,9 +469,7 @@
       <c r="V10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W10" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -503,9 +502,24 @@
       <c r="L11" s="7" t="n">
         <v>0.346430250383241</v>
       </c>
+      <c r="N11" s="7" t="n">
+        <v>0.0705074759334666</v>
+      </c>
+      <c r="O11" s="7" t="n">
+        <v>0.658905914059872</v>
+      </c>
       <c r="P11" s="7" t="n">
-        <v>0.016370896184561</v>
-      </c>
+        <v>0.008</v>
+      </c>
+      <c r="Q11" s="7" t="n">
+        <v>0.0065483584738244</v>
+      </c>
+      <c r="S11" s="8" t="n">
+        <v>0.398379320279884</v>
+      </c>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -538,9 +552,24 @@
       <c r="L12" s="7" t="n">
         <v>0.416788322028913</v>
       </c>
+      <c r="N12" s="7" t="n">
+        <v>0.0887285283104392</v>
+      </c>
+      <c r="O12" s="7" t="n">
+        <v>0.70695674067076</v>
+      </c>
       <c r="P12" s="7" t="n">
         <v>0.0103937990973635</v>
       </c>
+      <c r="Q12" s="7" t="n">
+        <v>0.0110895996480718</v>
+      </c>
+      <c r="S12" s="8" t="n">
+        <v>0.403477999822657</v>
+      </c>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -573,9 +602,24 @@
       <c r="L13" s="7" t="n">
         <v>0.490848270628325</v>
       </c>
+      <c r="N13" s="7" t="n">
+        <v>0.103274767135147</v>
+      </c>
+      <c r="O13" s="7" t="n">
+        <v>0.697672894095115</v>
+      </c>
       <c r="P13" s="7" t="n">
         <v>0.0251880200979944</v>
       </c>
+      <c r="Q13" s="7" t="n">
+        <v>0.0448458379282983</v>
+      </c>
+      <c r="S13" s="8" t="n">
+        <v>0.427328213718856</v>
+      </c>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -608,9 +652,24 @@
       <c r="L14" s="7" t="n">
         <v>0.557705909277033</v>
       </c>
+      <c r="N14" s="7" t="n">
+        <v>0.129799387310815</v>
+      </c>
+      <c r="O14" s="7" t="n">
+        <v>0.730748337429236</v>
+      </c>
       <c r="P14" s="7" t="n">
         <v>0.139945361418232</v>
       </c>
+      <c r="Q14" s="7" t="n">
+        <v>0.0851512581645233</v>
+      </c>
+      <c r="S14" s="8" t="n">
+        <v>0.460075512612307</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -643,9 +702,24 @@
       <c r="L15" s="7" t="n">
         <v>0.61100264429743</v>
       </c>
+      <c r="N15" s="7" t="n">
+        <v>0.165530081284066</v>
+      </c>
+      <c r="O15" s="7" t="n">
+        <v>0.857778041413194</v>
+      </c>
       <c r="P15" s="7" t="n">
         <v>0.460469833473239</v>
       </c>
+      <c r="Q15" s="7" t="n">
+        <v>0.102083371666269</v>
+      </c>
+      <c r="S15" s="8" t="n">
+        <v>0.542780715495995</v>
+      </c>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -678,9 +752,24 @@
       <c r="L16" s="7" t="n">
         <v>0.644988051611281</v>
       </c>
+      <c r="N16" s="7" t="n">
+        <v>0.196828844969069</v>
+      </c>
+      <c r="O16" s="7" t="n">
+        <v>0.937922807749506</v>
+      </c>
       <c r="P16" s="7" t="n">
         <v>0.903321814436053</v>
       </c>
+      <c r="Q16" s="7" t="n">
+        <v>0.0829409093861648</v>
+      </c>
+      <c r="S16" s="8" t="n">
+        <v>0.597245759232133</v>
+      </c>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -713,9 +802,24 @@
       <c r="L17" s="7" t="n">
         <v>0.656189328703893</v>
       </c>
+      <c r="N17" s="7" t="n">
+        <v>0.256848942185297</v>
+      </c>
+      <c r="O17" s="7" t="n">
+        <v>0.971790482932668</v>
+      </c>
       <c r="P17" s="7" t="n">
         <v>0.896915279740246</v>
       </c>
+      <c r="Q17" s="7" t="n">
+        <v>0.0597791180143377</v>
+      </c>
+      <c r="S17" s="8" t="n">
+        <v>0.575035224977795</v>
+      </c>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -748,9 +852,24 @@
       <c r="L18" s="7" t="n">
         <v>0.626682334894627</v>
       </c>
+      <c r="N18" s="7" t="n">
+        <v>0.317381530829239</v>
+      </c>
+      <c r="O18" s="7" t="n">
+        <v>1</v>
+      </c>
       <c r="P18" s="7" t="n">
         <v>0.621909418641324</v>
       </c>
+      <c r="Q18" s="7" t="n">
+        <v>0.0491574047087697</v>
+      </c>
+      <c r="S18" s="8" t="n">
+        <v>0.54509465887086</v>
+      </c>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -783,9 +902,24 @@
       <c r="L19" s="7" t="n">
         <v>0.568268656883698</v>
       </c>
+      <c r="N19" s="7" t="n">
+        <v>0.415346602102964</v>
+      </c>
+      <c r="O19" s="7" t="n">
+        <v>0.977379439764912</v>
+      </c>
       <c r="P19" s="7" t="n">
         <v>0.457528218029069</v>
       </c>
+      <c r="Q19" s="7" t="n">
+        <v>0.0461270214933403</v>
+      </c>
+      <c r="S19" s="8" t="n">
+        <v>0.530354970947356</v>
+      </c>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -818,9 +952,24 @@
       <c r="L20" s="7" t="n">
         <v>0.47928628294386</v>
       </c>
+      <c r="N20" s="7" t="n">
+        <v>0.552412036229223</v>
+      </c>
+      <c r="O20" s="7" t="n">
+        <v>0.950685718706692</v>
+      </c>
       <c r="P20" s="7" t="n">
         <v>0.352277986466237</v>
       </c>
+      <c r="Q20" s="7" t="n">
+        <v>0.0563372107354287</v>
+      </c>
+      <c r="S20" s="8" t="n">
+        <v>0.528019414149809</v>
+      </c>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -853,9 +1002,24 @@
       <c r="L21" s="7" t="n">
         <v>0.377446822825637</v>
       </c>
+      <c r="N21" s="7" t="n">
+        <v>0.639113582111387</v>
+      </c>
+      <c r="O21" s="7" t="n">
+        <v>0.958970591177611</v>
+      </c>
       <c r="P21" s="7" t="n">
         <v>0.337618244442143</v>
       </c>
+      <c r="Q21" s="7" t="n">
+        <v>0.101440113510113</v>
+      </c>
+      <c r="S21" s="8" t="n">
+        <v>0.540006981175897</v>
+      </c>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -888,9 +1052,24 @@
       <c r="L22" s="7" t="n">
         <v>0.278314248490297</v>
       </c>
+      <c r="N22" s="7" t="n">
+        <v>0.674338462633188</v>
+      </c>
+      <c r="O22" s="7" t="n">
+        <v>0.93084264191956</v>
+      </c>
       <c r="P22" s="7" t="n">
         <v>0.405277559343489</v>
       </c>
+      <c r="Q22" s="7" t="n">
+        <v>0.192009987120836</v>
+      </c>
+      <c r="S22" s="8" t="n">
+        <v>0.560750214554387</v>
+      </c>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -923,9 +1102,24 @@
       <c r="L23" s="7" t="n">
         <v>0.197682378555147</v>
       </c>
+      <c r="N23" s="7" t="n">
+        <v>0.740652437515367</v>
+      </c>
+      <c r="O23" s="7" t="n">
+        <v>0.914290010115263</v>
+      </c>
       <c r="P23" s="7" t="n">
         <v>0.494187288283169</v>
       </c>
+      <c r="Q23" s="7" t="n">
+        <v>0.404636436487972</v>
+      </c>
+      <c r="S23" s="8" t="n">
+        <v>0.620727773414092</v>
+      </c>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -958,9 +1152,24 @@
       <c r="L24" s="7" t="n">
         <v>0.14269362629405</v>
       </c>
+      <c r="N24" s="7" t="n">
+        <v>0.823981268448678</v>
+      </c>
+      <c r="O24" s="7" t="n">
+        <v>0.952218556619864</v>
+      </c>
       <c r="P24" s="7" t="n">
         <v>0.526601186258332</v>
       </c>
+      <c r="Q24" s="7" t="n">
+        <v>0.639285435683747</v>
+      </c>
+      <c r="S24" s="8" t="n">
+        <v>0.721469070635879</v>
+      </c>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -993,9 +1202,24 @@
       <c r="L25" s="7" t="n">
         <v>0.103891990157726</v>
       </c>
+      <c r="N25" s="7" t="n">
+        <v>0.824520346067591</v>
+      </c>
+      <c r="O25" s="7" t="n">
+        <v>0.95073381245413</v>
+      </c>
       <c r="P25" s="7" t="n">
         <v>0.534129846277637</v>
       </c>
+      <c r="Q25" s="7" t="n">
+        <v>0.807695218326087</v>
+      </c>
+      <c r="S25" s="8" t="n">
+        <v>0.780654508270583</v>
+      </c>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1028,9 +1252,24 @@
       <c r="L26" s="7" t="n">
         <v>0.0731849039024679</v>
       </c>
+      <c r="N26" s="7" t="n">
+        <v>0.826192388055591</v>
+      </c>
+      <c r="O26" s="7" t="n">
+        <v>0.941964793843153</v>
+      </c>
       <c r="P26" s="7" t="n">
         <v>0.527093704782073</v>
       </c>
+      <c r="Q26" s="7" t="n">
+        <v>0.90807202995341</v>
+      </c>
+      <c r="S26" s="8" t="n">
+        <v>0.789316623055342</v>
+      </c>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -1063,9 +1302,24 @@
       <c r="L27" s="7" t="n">
         <v>0.0505387387422169</v>
       </c>
+      <c r="N27" s="7" t="n">
+        <v>0.860905911663345</v>
+      </c>
+      <c r="O27" s="7" t="n">
+        <v>0.922078352834891</v>
+      </c>
       <c r="P27" s="7" t="n">
         <v>0.513878155201865</v>
       </c>
+      <c r="Q27" s="7" t="n">
+        <v>0.940914816032929</v>
+      </c>
+      <c r="S27" s="8" t="n">
+        <v>0.781185383141206</v>
+      </c>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1098,9 +1352,24 @@
       <c r="L28" s="7" t="n">
         <v>0.037297987892821</v>
       </c>
+      <c r="N28" s="7" t="n">
+        <v>0.943145048779266</v>
+      </c>
+      <c r="O28" s="7" t="n">
+        <v>0.904179099867514</v>
+      </c>
       <c r="P28" s="7" t="n">
         <v>0.475865348199019</v>
       </c>
+      <c r="Q28" s="7" t="n">
+        <v>0.937915315810007</v>
+      </c>
+      <c r="S28" s="8" t="n">
+        <v>0.818592626200122</v>
+      </c>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1133,9 +1402,24 @@
       <c r="L29" s="7" t="n">
         <v>0.0232219215809231</v>
       </c>
+      <c r="N29" s="7" t="n">
+        <v>0.969525134581981</v>
+      </c>
+      <c r="O29" s="7" t="n">
+        <v>0.864561964337502</v>
+      </c>
       <c r="P29" s="7" t="n">
         <v>0.419015424083027</v>
       </c>
+      <c r="Q29" s="7" t="n">
+        <v>0.884292175520252</v>
+      </c>
+      <c r="S29" s="8" t="n">
+        <v>0.832479335072554</v>
+      </c>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1168,9 +1452,24 @@
       <c r="L30" s="7" t="n">
         <v>0.0244550478900452</v>
       </c>
+      <c r="N30" s="7" t="n">
+        <v>0.935990430168677</v>
+      </c>
+      <c r="O30" s="7" t="n">
+        <v>0.869621171548307</v>
+      </c>
       <c r="P30" s="7" t="n">
         <v>0.365583356042107</v>
       </c>
+      <c r="Q30" s="7" t="n">
+        <v>0.813878620534493</v>
+      </c>
+      <c r="S30" s="8" t="n">
+        <v>0.64621101633684</v>
+      </c>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1203,9 +1502,24 @@
       <c r="L31" s="7" t="n">
         <v>0.0164695987143855</v>
       </c>
+      <c r="N31" s="7" t="n">
+        <v>0.901722692399693</v>
+      </c>
+      <c r="O31" s="7" t="n">
+        <v>0.899248988379464</v>
+      </c>
       <c r="P31" s="7" t="n">
         <v>0.313395779960234</v>
       </c>
+      <c r="Q31" s="7" t="n">
+        <v>0.749526414320907</v>
+      </c>
+      <c r="S31" s="8" t="n">
+        <v>0.420219323346586</v>
+      </c>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -1238,9 +1552,24 @@
       <c r="L32" s="7" t="n">
         <v>0.0189289709716995</v>
       </c>
+      <c r="N32" s="7" t="n">
+        <v>0.907315140549089</v>
+      </c>
+      <c r="O32" s="7" t="n">
+        <v>0.898931676004229</v>
+      </c>
       <c r="P32" s="7" t="n">
         <v>0.26755065212131</v>
       </c>
+      <c r="Q32" s="7" t="n">
+        <v>0.678372190100115</v>
+      </c>
+      <c r="S32" s="8" t="n">
+        <v>0.296813063501133</v>
+      </c>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1273,9 +1602,24 @@
       <c r="L33" s="7" t="n">
         <v>0.0157497844449936</v>
       </c>
+      <c r="N33" s="7" t="n">
+        <v>0.948803801844635</v>
+      </c>
+      <c r="O33" s="7" t="n">
+        <v>0.884814779054237</v>
+      </c>
       <c r="P33" s="7" t="n">
         <v>0.220729193242084</v>
       </c>
+      <c r="Q33" s="7" t="n">
+        <v>0.609624964202489</v>
+      </c>
+      <c r="S33" s="8" t="n">
+        <v>0.241008578448887</v>
+      </c>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -1308,9 +1652,24 @@
       <c r="L34" s="7" t="n">
         <v>0.0206806794300947</v>
       </c>
+      <c r="N34" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="7" t="n">
+        <v>0.874592063821858</v>
+      </c>
       <c r="P34" s="7" t="n">
         <v>0.174859712409798</v>
       </c>
+      <c r="Q34" s="7" t="n">
+        <v>0.529109461234866</v>
+      </c>
+      <c r="S34" s="8" t="n">
+        <v>0.198060927324944</v>
+      </c>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1343,9 +1702,24 @@
       <c r="L35" s="7" t="n">
         <v>0.0259998008416251</v>
       </c>
+      <c r="N35" s="7" t="n">
+        <v>0.979902823118686</v>
+      </c>
+      <c r="O35" s="7" t="n">
+        <v>0.870455180672695</v>
+      </c>
       <c r="P35" s="7" t="n">
         <v>0.140151972150759</v>
       </c>
+      <c r="Q35" s="7" t="n">
+        <v>0.4503980448556</v>
+      </c>
+      <c r="S35" s="8" t="n">
+        <v>0.179366126106183</v>
+      </c>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -1378,9 +1752,24 @@
       <c r="L36" s="7" t="n">
         <v>0.0531843805350936</v>
       </c>
+      <c r="N36" s="7" t="n">
+        <v>0.914420792058838</v>
+      </c>
+      <c r="O36" s="7" t="n">
+        <v>0.863979425238946</v>
+      </c>
       <c r="P36" s="7" t="n">
         <v>0.106942388195053</v>
       </c>
+      <c r="Q36" s="7" t="n">
+        <v>0.368557604778562</v>
+      </c>
+      <c r="S36" s="8" t="n">
+        <v>0.170673773202596</v>
+      </c>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -1413,9 +1802,24 @@
       <c r="L37" s="7" t="n">
         <v>0.0644042852666233</v>
       </c>
+      <c r="N37" s="7" t="n">
+        <v>0.860631718914122</v>
+      </c>
+      <c r="O37" s="7" t="n">
+        <v>0.855765080575428</v>
+      </c>
       <c r="P37" s="7" t="n">
-        <v>0.0512496252183468</v>
-      </c>
+        <v>0.0775</v>
+      </c>
+      <c r="Q37" s="7" t="n">
+        <v>0.292754567721736</v>
+      </c>
+      <c r="S37" s="8" t="n">
+        <v>0.163625001571542</v>
+      </c>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -1448,9 +1852,24 @@
       <c r="L38" s="7" t="n">
         <v>0.075841808527235</v>
       </c>
+      <c r="N38" s="7" t="n">
+        <v>0.839585969920973</v>
+      </c>
+      <c r="O38" s="7" t="n">
+        <v>0.798786155943385</v>
+      </c>
       <c r="P38" s="7" t="n">
-        <v>0.0435009172789198</v>
-      </c>
+        <v>0.0557</v>
+      </c>
+      <c r="Q38" s="7" t="n">
+        <v>0.224743213015529</v>
+      </c>
+      <c r="S38" s="8" t="n">
+        <v>0.154690651582248</v>
+      </c>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -1483,9 +1902,24 @@
       <c r="L39" s="7" t="n">
         <v>0.0820258920643171</v>
       </c>
+      <c r="N39" s="7" t="n">
+        <v>0.848252595938346</v>
+      </c>
+      <c r="O39" s="7" t="n">
+        <v>0.728409011168105</v>
+      </c>
       <c r="P39" s="7" t="n">
-        <v>0.0222300155212269</v>
-      </c>
+        <v>0.04</v>
+      </c>
+      <c r="Q39" s="7" t="n">
+        <v>0.167817229522706</v>
+      </c>
+      <c r="S39" s="8" t="n">
+        <v>0.146112807824047</v>
+      </c>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -1518,9 +1952,24 @@
       <c r="L40" s="7" t="n">
         <v>0.0838830338412939</v>
       </c>
+      <c r="N40" s="7" t="n">
+        <v>0.840737369376341</v>
+      </c>
+      <c r="O40" s="7" t="n">
+        <v>0.722849714895435</v>
+      </c>
       <c r="P40" s="7" t="n">
         <v>0.0335601115254911</v>
       </c>
+      <c r="Q40" s="7" t="n">
+        <v>0.124138464092599</v>
+      </c>
+      <c r="S40" s="8" t="n">
+        <v>0.1360857067652</v>
+      </c>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -1553,9 +2002,24 @@
       <c r="L41" s="7" t="n">
         <v>0.0785235033927056</v>
       </c>
+      <c r="N41" s="7" t="n">
+        <v>0.818943767751521</v>
+      </c>
+      <c r="O41" s="7" t="n">
+        <v>0.772714066529342</v>
+      </c>
       <c r="P41" s="7" t="n">
         <v>0.026965419186884</v>
       </c>
+      <c r="Q41" s="7" t="n">
+        <v>0.091244250683987</v>
+      </c>
+      <c r="S41" s="8" t="n">
+        <v>0.128376730137942</v>
+      </c>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -1588,9 +2052,24 @@
       <c r="L42" s="7" t="n">
         <v>0.0728734241218842</v>
       </c>
+      <c r="N42" s="7" t="n">
+        <v>0.751701955257871</v>
+      </c>
+      <c r="O42" s="7" t="n">
+        <v>0.697808447809728</v>
+      </c>
       <c r="P42" s="7" t="n">
         <v>0.015263054258194</v>
       </c>
+      <c r="Q42" s="7" t="n">
+        <v>0.0676692816640285</v>
+      </c>
+      <c r="S42" s="8" t="n">
+        <v>0.120831515439488</v>
+      </c>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -1623,9 +2102,24 @@
       <c r="L43" s="7" t="n">
         <v>0.0604581863492757</v>
       </c>
+      <c r="N43" s="7" t="n">
+        <v>0.679461962784371</v>
+      </c>
+      <c r="O43" s="7" t="n">
+        <v>0.650566847044003</v>
+      </c>
       <c r="P43" s="7" t="n">
         <v>0.0159800180658007</v>
       </c>
+      <c r="Q43" s="7" t="n">
+        <v>0.0509463747798478</v>
+      </c>
+      <c r="S43" s="8" t="n">
+        <v>0.118877338566591</v>
+      </c>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1658,9 +2152,24 @@
       <c r="L44" s="7" t="n">
         <v>0.0531814921272853</v>
       </c>
+      <c r="N44" s="7" t="n">
+        <v>0.629617707843639</v>
+      </c>
+      <c r="O44" s="7" t="n">
+        <v>0.694056990729689</v>
+      </c>
       <c r="P44" s="7" t="n">
         <v>0.0127715383741411</v>
       </c>
+      <c r="Q44" s="7" t="n">
+        <v>0.0393466732843488</v>
+      </c>
+      <c r="S44" s="8" t="n">
+        <v>0.120702624066909</v>
+      </c>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -1693,9 +2202,24 @@
       <c r="L45" s="7" t="n">
         <v>0.0531814001066711</v>
       </c>
+      <c r="N45" s="7" t="n">
+        <v>0.589318256470762</v>
+      </c>
+      <c r="O45" s="7" t="n">
+        <v>0.731576447572711</v>
+      </c>
       <c r="P45" s="7" t="n">
         <v>0.0130988747085952</v>
       </c>
+      <c r="Q45" s="7" t="n">
+        <v>0.0267572018466478</v>
+      </c>
+      <c r="S45" s="8" t="n">
+        <v>0.131629825835622</v>
+      </c>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -1728,9 +2252,24 @@
       <c r="L46" s="7" t="n">
         <v>0.0541073769397165</v>
       </c>
+      <c r="N46" s="7" t="n">
+        <v>0.557612725716759</v>
+      </c>
+      <c r="O46" s="7" t="n">
+        <v>0.666250757546469</v>
+      </c>
       <c r="P46" s="7" t="n">
         <v>0.00364263525613273</v>
       </c>
+      <c r="Q46" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" s="8" t="n">
+        <v>0.145608679608511</v>
+      </c>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -1763,9 +2302,24 @@
       <c r="L47" s="7" t="n">
         <v>0.0604230011743034</v>
       </c>
+      <c r="N47" s="7" t="n">
+        <v>0.533625665683436</v>
+      </c>
+      <c r="O47" s="7" t="n">
+        <v>0.513710345932646</v>
+      </c>
       <c r="P47" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q47" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" s="8" t="n">
+        <v>0.150160848603993</v>
+      </c>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -1798,9 +2352,24 @@
       <c r="L48" s="7" t="n">
         <v>0.0945890984610229</v>
       </c>
+      <c r="N48" s="7" t="n">
+        <v>0.491686417317698</v>
+      </c>
+      <c r="O48" s="7" t="n">
+        <v>0.668040864058981</v>
+      </c>
       <c r="P48" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q48" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" s="8" t="n">
+        <v>0.14703819913371</v>
+      </c>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -1833,9 +2402,24 @@
       <c r="L49" s="7" t="n">
         <v>0.179551862206952</v>
       </c>
+      <c r="N49" s="7" t="n">
+        <v>0.439957311206778</v>
+      </c>
+      <c r="O49" s="7" t="n">
+        <v>0.679525056536049</v>
+      </c>
       <c r="P49" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q49" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" s="8" t="n">
+        <v>0.140375693804613</v>
+      </c>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1868,9 +2452,24 @@
       <c r="L50" s="7" t="n">
         <v>0.299982581310992</v>
       </c>
+      <c r="N50" s="7" t="n">
+        <v>0.374128901490533</v>
+      </c>
+      <c r="O50" s="7" t="n">
+        <v>0.660678946184692</v>
+      </c>
       <c r="P50" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q50" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" s="8" t="n">
+        <v>0.139668272631271</v>
+      </c>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -1903,9 +2502,24 @@
       <c r="L51" s="7" t="n">
         <v>0.438296380776138</v>
       </c>
+      <c r="N51" s="7" t="n">
+        <v>0.334923840517699</v>
+      </c>
+      <c r="O51" s="7" t="n">
+        <v>0.626912068759043</v>
+      </c>
       <c r="P51" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q51" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" s="8" t="n">
+        <v>0.144520956268633</v>
+      </c>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -1938,9 +2552,24 @@
       <c r="L52" s="7" t="n">
         <v>0.518200293275087</v>
       </c>
+      <c r="N52" s="7" t="n">
+        <v>0.320910344351199</v>
+      </c>
+      <c r="O52" s="7" t="n">
+        <v>0.536910526516458</v>
+      </c>
       <c r="P52" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q52" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" s="8" t="n">
+        <v>0.154433556530129</v>
+      </c>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -1973,9 +2602,24 @@
       <c r="L53" s="7" t="n">
         <v>0.525901637744971</v>
       </c>
+      <c r="N53" s="7" t="n">
+        <v>0.291143720076843</v>
+      </c>
+      <c r="O53" s="7" t="n">
+        <v>0.513655751591967</v>
+      </c>
       <c r="P53" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q53" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" s="8" t="n">
+        <v>0.161665656377309</v>
+      </c>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -2008,9 +2652,24 @@
       <c r="L54" s="7" t="n">
         <v>0.485539144158582</v>
       </c>
+      <c r="N54" s="7" t="n">
+        <v>0.27356808782089</v>
+      </c>
+      <c r="O54" s="7" t="n">
+        <v>0.557766332837266</v>
+      </c>
       <c r="P54" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q54" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" s="8" t="n">
+        <v>0.165803035708245</v>
+      </c>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -2043,9 +2702,24 @@
       <c r="L55" s="7" t="n">
         <v>0.444136921087233</v>
       </c>
+      <c r="N55" s="7" t="n">
+        <v>0.251415267380195</v>
+      </c>
+      <c r="O55" s="7" t="n">
+        <v>0.588340186331177</v>
+      </c>
       <c r="P55" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q55" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" s="8" t="n">
+        <v>0.168930987356168</v>
+      </c>
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -2078,9 +2752,24 @@
       <c r="L56" s="7" t="n">
         <v>0.429870281607446</v>
       </c>
+      <c r="N56" s="7" t="n">
+        <v>0.233206967491043</v>
+      </c>
+      <c r="O56" s="7" t="n">
+        <v>0.594024183076204</v>
+      </c>
       <c r="P56" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q56" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S56" s="8" t="n">
+        <v>0.168676308401356</v>
+      </c>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -2113,9 +2802,24 @@
       <c r="L57" s="7" t="n">
         <v>0.428329914823626</v>
       </c>
+      <c r="N57" s="7" t="n">
+        <v>0.21484621566543</v>
+      </c>
+      <c r="O57" s="7" t="n">
+        <v>0.588141050816057</v>
+      </c>
       <c r="P57" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q57" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" s="8" t="n">
+        <v>0.174695960335137</v>
+      </c>
+      <c r="T57" s="8"/>
+      <c r="U57" s="8"/>
+      <c r="V57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -2148,9 +2852,24 @@
       <c r="L58" s="7" t="n">
         <v>0.41403845328492</v>
       </c>
+      <c r="N58" s="7" t="n">
+        <v>0.193030705087291</v>
+      </c>
+      <c r="O58" s="7" t="n">
+        <v>0.57504071711158</v>
+      </c>
       <c r="P58" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q58" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" s="8" t="n">
+        <v>0.181444562174254</v>
+      </c>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -2183,9 +2902,24 @@
       <c r="L59" s="7" t="n">
         <v>0.377914844511759</v>
       </c>
+      <c r="N59" s="7" t="n">
+        <v>0.169973827333954</v>
+      </c>
+      <c r="O59" s="7" t="n">
+        <v>0.543397763355008</v>
+      </c>
       <c r="P59" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q59" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" s="8" t="n">
+        <v>0.187295386017967</v>
+      </c>
+      <c r="T59" s="8"/>
+      <c r="U59" s="8"/>
+      <c r="V59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -2218,9 +2952,24 @@
       <c r="L60" s="7" t="n">
         <v>0.337158050919218</v>
       </c>
+      <c r="N60" s="7" t="n">
+        <v>0.156261387178316</v>
+      </c>
+      <c r="O60" s="7" t="n">
+        <v>0.505792569089049</v>
+      </c>
       <c r="P60" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q60" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" s="8" t="n">
+        <v>0.190661877248146</v>
+      </c>
+      <c r="T60" s="8"/>
+      <c r="U60" s="8"/>
+      <c r="V60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -2253,9 +3002,24 @@
       <c r="L61" s="7" t="n">
         <v>0.299226580006317</v>
       </c>
+      <c r="N61" s="7" t="n">
+        <v>0.145320517707134</v>
+      </c>
+      <c r="O61" s="7" t="n">
+        <v>0.447164833935561</v>
+      </c>
       <c r="P61" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q61" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" s="8" t="n">
+        <v>0.197867325085204</v>
+      </c>
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -2288,9 +3052,24 @@
       <c r="L62" s="7" t="n">
         <v>0.271067025852657</v>
       </c>
+      <c r="N62" s="7" t="n">
+        <v>0.126422078682253</v>
+      </c>
+      <c r="O62" s="7" t="n">
+        <v>0.41752939548792</v>
+      </c>
       <c r="P62" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q62" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" s="8" t="n">
+        <v>0.200744296433752</v>
+      </c>
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+      <c r="V62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -2323,9 +3102,24 @@
       <c r="L63" s="7" t="n">
         <v>0.240125150087756</v>
       </c>
+      <c r="N63" s="7" t="n">
+        <v>0.108467361331286</v>
+      </c>
+      <c r="O63" s="7" t="n">
+        <v>0.302382172799922</v>
+      </c>
       <c r="P63" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q63" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S63" s="8" t="n">
+        <v>0.202169683703366</v>
+      </c>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -2358,9 +3152,24 @@
       <c r="L64" s="7" t="n">
         <v>0.220382381808246</v>
       </c>
+      <c r="N64" s="7" t="n">
+        <v>0.0902841200251656</v>
+      </c>
+      <c r="O64" s="7" t="n">
+        <v>0.204330626082583</v>
+      </c>
       <c r="P64" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q64" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" s="8" t="n">
+        <v>0.200806669778084</v>
+      </c>
+      <c r="T64" s="8"/>
+      <c r="U64" s="8"/>
+      <c r="V64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -2393,9 +3202,24 @@
       <c r="L65" s="7" t="n">
         <v>0.19423312426359</v>
       </c>
+      <c r="N65" s="7" t="n">
+        <v>0.0772031251773838</v>
+      </c>
+      <c r="O65" s="7" t="n">
+        <v>0.188233495674414</v>
+      </c>
       <c r="P65" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q65" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S65" s="8" t="n">
+        <v>0.197315610088285</v>
+      </c>
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -2428,9 +3252,24 @@
       <c r="L66" s="7" t="n">
         <v>0.16965743152827</v>
       </c>
+      <c r="N66" s="7" t="n">
+        <v>0.0712117522095793</v>
+      </c>
+      <c r="O66" s="7" t="n">
+        <v>0.254318884400522</v>
+      </c>
       <c r="P66" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q66" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" s="8" t="n">
+        <v>0.193508058641756</v>
+      </c>
+      <c r="T66" s="8"/>
+      <c r="U66" s="8"/>
+      <c r="V66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -2463,9 +3302,24 @@
       <c r="L67" s="7" t="n">
         <v>0.148959127396155</v>
       </c>
+      <c r="N67" s="7" t="n">
+        <v>0.0650747091443748</v>
+      </c>
+      <c r="O67" s="7" t="n">
+        <v>0.321641815035715</v>
+      </c>
       <c r="P67" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q67" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" s="8" t="n">
+        <v>0.190664547845022</v>
+      </c>
+      <c r="T67" s="8"/>
+      <c r="U67" s="8"/>
+      <c r="V67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -2498,9 +3352,24 @@
       <c r="L68" s="7" t="n">
         <v>0.129854202209054</v>
       </c>
+      <c r="N68" s="7" t="n">
+        <v>0.057786055619086</v>
+      </c>
+      <c r="O68" s="7" t="n">
+        <v>0.374246578201715</v>
+      </c>
       <c r="P68" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q68" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" s="8" t="n">
+        <v>0.183088741789439</v>
+      </c>
+      <c r="T68" s="8"/>
+      <c r="U68" s="8"/>
+      <c r="V68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -2533,9 +3402,24 @@
       <c r="L69" s="7" t="n">
         <v>0.112751040672247</v>
       </c>
+      <c r="N69" s="7" t="n">
+        <v>0.0558592458274331</v>
+      </c>
+      <c r="O69" s="7" t="n">
+        <v>0.418448448242297</v>
+      </c>
       <c r="P69" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q69" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" s="8" t="n">
+        <v>0.178312827007274</v>
+      </c>
+      <c r="T69" s="8"/>
+      <c r="U69" s="8"/>
+      <c r="V69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -2568,9 +3452,24 @@
       <c r="L70" s="7" t="n">
         <v>0.0963916885700926</v>
       </c>
+      <c r="N70" s="7" t="n">
+        <v>0.0505347059654789</v>
+      </c>
+      <c r="O70" s="7" t="n">
+        <v>0.449218142424956</v>
+      </c>
       <c r="P70" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q70" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" s="8" t="n">
+        <v>0.172019845644173</v>
+      </c>
+      <c r="T70" s="8"/>
+      <c r="U70" s="8"/>
+      <c r="V70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -2603,16 +3502,31 @@
       <c r="L71" s="7" t="n">
         <v>0.0777712699394244</v>
       </c>
+      <c r="N71" s="7" t="n">
+        <v>0.047004979874693</v>
+      </c>
+      <c r="O71" s="7" t="n">
+        <v>0.448775248054037</v>
+      </c>
       <c r="P71" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="Q71" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" s="8" t="n">
+        <v>0.164221111235425</v>
+      </c>
+      <c r="T71" s="8"/>
+      <c r="U71" s="8"/>
+      <c r="V71" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="I9:L9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="S9:V9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
[DrSpot] Add rest of SpO2 PPG spectra
</commit_message>
<xml_diff>
--- a/vitals_collection/drspot/docs/pulse_signature_vector.xlsx
+++ b/vitals_collection/drspot/docs/pulse_signature_vector.xlsx
@@ -262,10 +262,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="10" topLeftCell="B11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="T71" activeCellId="0" sqref="T71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="Q11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="11:11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -517,9 +519,15 @@
       <c r="S11" s="8" t="n">
         <v>0.398379320279884</v>
       </c>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
+      <c r="T11" s="8" t="n">
+        <v>0.388697613267937</v>
+      </c>
+      <c r="U11" s="8" t="n">
+        <v>0.391728998115649</v>
+      </c>
+      <c r="V11" s="8" t="n">
+        <v>0.390352380617476</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -567,9 +575,15 @@
       <c r="S12" s="8" t="n">
         <v>0.403477999822657</v>
       </c>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
+      <c r="T12" s="8" t="n">
+        <v>0.400262881015606</v>
+      </c>
+      <c r="U12" s="8" t="n">
+        <v>0.402519770909572</v>
+      </c>
+      <c r="V12" s="8" t="n">
+        <v>0.403919439509603</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -617,9 +631,15 @@
       <c r="S13" s="8" t="n">
         <v>0.427328213718856</v>
       </c>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
+      <c r="T13" s="8" t="n">
+        <v>0.429778241207729</v>
+      </c>
+      <c r="U13" s="8" t="n">
+        <v>0.426694058719735</v>
+      </c>
+      <c r="V13" s="8" t="n">
+        <v>0.428966661503996</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -667,9 +687,15 @@
       <c r="S14" s="8" t="n">
         <v>0.460075512612307</v>
       </c>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
+      <c r="T14" s="8" t="n">
+        <v>0.465648683692535</v>
+      </c>
+      <c r="U14" s="8" t="n">
+        <v>0.472550648121128</v>
+      </c>
+      <c r="V14" s="8" t="n">
+        <v>0.490179533266721</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -717,9 +743,15 @@
       <c r="S15" s="8" t="n">
         <v>0.542780715495995</v>
       </c>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
+      <c r="T15" s="8" t="n">
+        <v>0.551672772316695</v>
+      </c>
+      <c r="U15" s="8" t="n">
+        <v>0.558597221434521</v>
+      </c>
+      <c r="V15" s="8" t="n">
+        <v>0.568316443412054</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -767,9 +799,15 @@
       <c r="S16" s="8" t="n">
         <v>0.597245759232133</v>
       </c>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
+      <c r="T16" s="8" t="n">
+        <v>0.602406078136805</v>
+      </c>
+      <c r="U16" s="8" t="n">
+        <v>0.601624385396986</v>
+      </c>
+      <c r="V16" s="8" t="n">
+        <v>0.604899175918738</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -817,9 +855,15 @@
       <c r="S17" s="8" t="n">
         <v>0.575035224977795</v>
       </c>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
+      <c r="T17" s="8" t="n">
+        <v>0.584249357806828</v>
+      </c>
+      <c r="U17" s="8" t="n">
+        <v>0.597040509190701</v>
+      </c>
+      <c r="V17" s="8" t="n">
+        <v>0.608364701574628</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -867,9 +911,15 @@
       <c r="S18" s="8" t="n">
         <v>0.54509465887086</v>
       </c>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
+      <c r="T18" s="8" t="n">
+        <v>0.563406574476269</v>
+      </c>
+      <c r="U18" s="8" t="n">
+        <v>0.579192103845881</v>
+      </c>
+      <c r="V18" s="8" t="n">
+        <v>0.594361203161495</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -917,9 +967,15 @@
       <c r="S19" s="8" t="n">
         <v>0.530354970947356</v>
       </c>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
+      <c r="T19" s="8" t="n">
+        <v>0.546445676373633</v>
+      </c>
+      <c r="U19" s="8" t="n">
+        <v>0.560058734443574</v>
+      </c>
+      <c r="V19" s="8" t="n">
+        <v>0.57493650873192</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -967,9 +1023,15 @@
       <c r="S20" s="8" t="n">
         <v>0.528019414149809</v>
       </c>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
+      <c r="T20" s="8" t="n">
+        <v>0.536735731174397</v>
+      </c>
+      <c r="U20" s="8" t="n">
+        <v>0.547241416780047</v>
+      </c>
+      <c r="V20" s="8" t="n">
+        <v>0.556320266966579</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -1017,9 +1079,15 @@
       <c r="S21" s="8" t="n">
         <v>0.540006981175897</v>
       </c>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
+      <c r="T21" s="8" t="n">
+        <v>0.54329790545146</v>
+      </c>
+      <c r="U21" s="8" t="n">
+        <v>0.546756983045502</v>
+      </c>
+      <c r="V21" s="8" t="n">
+        <v>0.551618014046287</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1067,9 +1135,15 @@
       <c r="S22" s="8" t="n">
         <v>0.560750214554387</v>
       </c>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
+      <c r="T22" s="8" t="n">
+        <v>0.556144492848315</v>
+      </c>
+      <c r="U22" s="8" t="n">
+        <v>0.555370774788576</v>
+      </c>
+      <c r="V22" s="8" t="n">
+        <v>0.550402945632612</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1117,9 +1191,15 @@
       <c r="S23" s="8" t="n">
         <v>0.620727773414092</v>
       </c>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
+      <c r="T23" s="8" t="n">
+        <v>0.612534610944435</v>
+      </c>
+      <c r="U23" s="8" t="n">
+        <v>0.61411290914253</v>
+      </c>
+      <c r="V23" s="8" t="n">
+        <v>0.608457426276319</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -1167,9 +1247,15 @@
       <c r="S24" s="8" t="n">
         <v>0.721469070635879</v>
       </c>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
+      <c r="T24" s="8" t="n">
+        <v>0.729352810856382</v>
+      </c>
+      <c r="U24" s="8" t="n">
+        <v>0.733990655537518</v>
+      </c>
+      <c r="V24" s="8" t="n">
+        <v>0.740287985622117</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -1217,9 +1303,15 @@
       <c r="S25" s="8" t="n">
         <v>0.780654508270583</v>
       </c>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
+      <c r="T25" s="8" t="n">
+        <v>0.787801483550552</v>
+      </c>
+      <c r="U25" s="8" t="n">
+        <v>0.791552942381319</v>
+      </c>
+      <c r="V25" s="8" t="n">
+        <v>0.796311924527198</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1267,9 +1359,15 @@
       <c r="S26" s="8" t="n">
         <v>0.789316623055342</v>
       </c>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
+      <c r="T26" s="8" t="n">
+        <v>0.78818770149211</v>
+      </c>
+      <c r="U26" s="8" t="n">
+        <v>0.787451348882009</v>
+      </c>
+      <c r="V26" s="8" t="n">
+        <v>0.782734398247796</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -1317,9 +1415,15 @@
       <c r="S27" s="8" t="n">
         <v>0.781185383141206</v>
       </c>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
+      <c r="T27" s="8" t="n">
+        <v>0.77007203769184</v>
+      </c>
+      <c r="U27" s="8" t="n">
+        <v>0.757896717380142</v>
+      </c>
+      <c r="V27" s="8" t="n">
+        <v>0.743684237541256</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1367,9 +1471,15 @@
       <c r="S28" s="8" t="n">
         <v>0.818592626200122</v>
       </c>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
+      <c r="T28" s="8" t="n">
+        <v>0.820808991677471</v>
+      </c>
+      <c r="U28" s="8" t="n">
+        <v>0.818640180832684</v>
+      </c>
+      <c r="V28" s="8" t="n">
+        <v>0.82279963896614</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1417,9 +1527,15 @@
       <c r="S29" s="8" t="n">
         <v>0.832479335072554</v>
       </c>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
+      <c r="T29" s="8" t="n">
+        <v>0.852108791363242</v>
+      </c>
+      <c r="U29" s="8" t="n">
+        <v>0.860349999823746</v>
+      </c>
+      <c r="V29" s="8" t="n">
+        <v>0.86799736581657</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1467,9 +1583,15 @@
       <c r="S30" s="8" t="n">
         <v>0.64621101633684</v>
       </c>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
+      <c r="T30" s="8" t="n">
+        <v>0.637203287753888</v>
+      </c>
+      <c r="U30" s="8" t="n">
+        <v>0.622597861825024</v>
+      </c>
+      <c r="V30" s="8" t="n">
+        <v>0.595422703328111</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1517,9 +1639,15 @@
       <c r="S31" s="8" t="n">
         <v>0.420219323346586</v>
       </c>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
+      <c r="T31" s="8" t="n">
+        <v>0.381241482636859</v>
+      </c>
+      <c r="U31" s="8" t="n">
+        <v>0.334045229938337</v>
+      </c>
+      <c r="V31" s="8" t="n">
+        <v>0.274252165400357</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -1567,9 +1695,15 @@
       <c r="S32" s="8" t="n">
         <v>0.296813063501133</v>
       </c>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
+      <c r="T32" s="8" t="n">
+        <v>0.256200262343734</v>
+      </c>
+      <c r="U32" s="8" t="n">
+        <v>0.218393223006568</v>
+      </c>
+      <c r="V32" s="8" t="n">
+        <v>0.176422006702897</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1617,9 +1751,15 @@
       <c r="S33" s="8" t="n">
         <v>0.241008578448887</v>
       </c>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
+      <c r="T33" s="8" t="n">
+        <v>0.201772503242573</v>
+      </c>
+      <c r="U33" s="8" t="n">
+        <v>0.1622983550755</v>
+      </c>
+      <c r="V33" s="8" t="n">
+        <v>0.118204561121282</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -1667,9 +1807,15 @@
       <c r="S34" s="8" t="n">
         <v>0.198060927324944</v>
       </c>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
+      <c r="T34" s="8" t="n">
+        <v>0.161608023918943</v>
+      </c>
+      <c r="U34" s="8" t="n">
+        <v>0.123772760246946</v>
+      </c>
+      <c r="V34" s="8" t="n">
+        <v>0.0822965787010872</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1717,9 +1863,15 @@
       <c r="S35" s="8" t="n">
         <v>0.179366126106183</v>
       </c>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
+      <c r="T35" s="8" t="n">
+        <v>0.144642997553972</v>
+      </c>
+      <c r="U35" s="8" t="n">
+        <v>0.106502121460859</v>
+      </c>
+      <c r="V35" s="8" t="n">
+        <v>0.0658148294142598</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -1767,9 +1919,15 @@
       <c r="S36" s="8" t="n">
         <v>0.170673773202596</v>
       </c>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
+      <c r="T36" s="8" t="n">
+        <v>0.135725972162894</v>
+      </c>
+      <c r="U36" s="8" t="n">
+        <v>0.0976719031582882</v>
+      </c>
+      <c r="V36" s="8" t="n">
+        <v>0.0561179618925236</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -1817,9 +1975,15 @@
       <c r="S37" s="8" t="n">
         <v>0.163625001571542</v>
       </c>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
+      <c r="T37" s="8" t="n">
+        <v>0.128204579666906</v>
+      </c>
+      <c r="U37" s="8" t="n">
+        <v>0.0907373323329066</v>
+      </c>
+      <c r="V37" s="8" t="n">
+        <v>0.0500365863111631</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -1867,9 +2031,15 @@
       <c r="S38" s="8" t="n">
         <v>0.154690651582248</v>
       </c>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
+      <c r="T38" s="8" t="n">
+        <v>0.123563942412983</v>
+      </c>
+      <c r="U38" s="8" t="n">
+        <v>0.0891580038502873</v>
+      </c>
+      <c r="V38" s="8" t="n">
+        <v>0.0515815129022028</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -1917,9 +2087,15 @@
       <c r="S39" s="8" t="n">
         <v>0.146112807824047</v>
       </c>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
+      <c r="T39" s="8" t="n">
+        <v>0.118967890999142</v>
+      </c>
+      <c r="U39" s="8" t="n">
+        <v>0.0891580110661925</v>
+      </c>
+      <c r="V39" s="8" t="n">
+        <v>0.0579311232543576</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -1967,9 +2143,15 @@
       <c r="S40" s="8" t="n">
         <v>0.1360857067652</v>
       </c>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
+      <c r="T40" s="8" t="n">
+        <v>0.112811077963829</v>
+      </c>
+      <c r="U40" s="8" t="n">
+        <v>0.0881342954939728</v>
+      </c>
+      <c r="V40" s="8" t="n">
+        <v>0.0617819427706645</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -2017,9 +2199,15 @@
       <c r="S41" s="8" t="n">
         <v>0.128376730137942</v>
       </c>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
+      <c r="T41" s="8" t="n">
+        <v>0.107193120633992</v>
+      </c>
+      <c r="U41" s="8" t="n">
+        <v>0.0864775637682056</v>
+      </c>
+      <c r="V41" s="8" t="n">
+        <v>0.0640912049877853</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -2067,9 +2255,15 @@
       <c r="S42" s="8" t="n">
         <v>0.120831515439488</v>
       </c>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
+      <c r="T42" s="8" t="n">
+        <v>0.105196947332417</v>
+      </c>
+      <c r="U42" s="8" t="n">
+        <v>0.0879365065494422</v>
+      </c>
+      <c r="V42" s="8" t="n">
+        <v>0.0704111242740344</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -2117,9 +2311,15 @@
       <c r="S43" s="8" t="n">
         <v>0.118877338566591</v>
       </c>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
+      <c r="T43" s="8" t="n">
+        <v>0.105277757529992</v>
+      </c>
+      <c r="U43" s="8" t="n">
+        <v>0.0923845247022863</v>
+      </c>
+      <c r="V43" s="8" t="n">
+        <v>0.0782162158412398</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -2167,9 +2367,15 @@
       <c r="S44" s="8" t="n">
         <v>0.120702624066909</v>
       </c>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="8"/>
+      <c r="T44" s="8" t="n">
+        <v>0.111101871208282</v>
+      </c>
+      <c r="U44" s="8" t="n">
+        <v>0.0983212841034687</v>
+      </c>
+      <c r="V44" s="8" t="n">
+        <v>0.0866907461488815</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -2217,9 +2423,15 @@
       <c r="S45" s="8" t="n">
         <v>0.131629825835622</v>
       </c>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="8"/>
+      <c r="T45" s="8" t="n">
+        <v>0.120208421312697</v>
+      </c>
+      <c r="U45" s="8" t="n">
+        <v>0.107071504461387</v>
+      </c>
+      <c r="V45" s="8" t="n">
+        <v>0.0940091912092553</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -2267,9 +2479,15 @@
       <c r="S46" s="8" t="n">
         <v>0.145608679608511</v>
       </c>
-      <c r="T46" s="8"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="8"/>
+      <c r="T46" s="8" t="n">
+        <v>0.130986540796109</v>
+      </c>
+      <c r="U46" s="8" t="n">
+        <v>0.116113508591282</v>
+      </c>
+      <c r="V46" s="8" t="n">
+        <v>0.100312018766281</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -2317,9 +2535,15 @@
       <c r="S47" s="8" t="n">
         <v>0.150160848603993</v>
       </c>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
+      <c r="T47" s="8" t="n">
+        <v>0.137383649709195</v>
+      </c>
+      <c r="U47" s="8" t="n">
+        <v>0.123701352309124</v>
+      </c>
+      <c r="V47" s="8" t="n">
+        <v>0.109519750092913</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -2367,9 +2591,15 @@
       <c r="S48" s="8" t="n">
         <v>0.14703819913371</v>
       </c>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="8"/>
+      <c r="T48" s="8" t="n">
+        <v>0.137423986569608</v>
+      </c>
+      <c r="U48" s="8" t="n">
+        <v>0.127735100515698</v>
+      </c>
+      <c r="V48" s="8" t="n">
+        <v>0.118023768436832</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -2417,9 +2647,15 @@
       <c r="S49" s="8" t="n">
         <v>0.140375693804613</v>
       </c>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="8"/>
+      <c r="T49" s="8" t="n">
+        <v>0.137420797228858</v>
+      </c>
+      <c r="U49" s="8" t="n">
+        <v>0.13217278262359</v>
+      </c>
+      <c r="V49" s="8" t="n">
+        <v>0.127095904599009</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -2467,9 +2703,15 @@
       <c r="S50" s="8" t="n">
         <v>0.139668272631271</v>
       </c>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="8"/>
+      <c r="T50" s="8" t="n">
+        <v>0.138296033736632</v>
+      </c>
+      <c r="U50" s="8" t="n">
+        <v>0.137115461636449</v>
+      </c>
+      <c r="V50" s="8" t="n">
+        <v>0.13474313350211</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -2517,9 +2759,15 @@
       <c r="S51" s="8" t="n">
         <v>0.144520956268633</v>
       </c>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
+      <c r="T51" s="8" t="n">
+        <v>0.145439447390704</v>
+      </c>
+      <c r="U51" s="8" t="n">
+        <v>0.144807028560957</v>
+      </c>
+      <c r="V51" s="8" t="n">
+        <v>0.144954874810767</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -2567,9 +2815,15 @@
       <c r="S52" s="8" t="n">
         <v>0.154433556530129</v>
       </c>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="8"/>
+      <c r="T52" s="8" t="n">
+        <v>0.154375538071529</v>
+      </c>
+      <c r="U52" s="8" t="n">
+        <v>0.15516989949208</v>
+      </c>
+      <c r="V52" s="8" t="n">
+        <v>0.158053745068484</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -2617,9 +2871,15 @@
       <c r="S53" s="8" t="n">
         <v>0.161665656377309</v>
       </c>
-      <c r="T53" s="8"/>
-      <c r="U53" s="8"/>
-      <c r="V53" s="8"/>
+      <c r="T53" s="8" t="n">
+        <v>0.162218800228477</v>
+      </c>
+      <c r="U53" s="8" t="n">
+        <v>0.165252197952388</v>
+      </c>
+      <c r="V53" s="8" t="n">
+        <v>0.167646690372851</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -2667,9 +2927,15 @@
       <c r="S54" s="8" t="n">
         <v>0.165803035708245</v>
       </c>
-      <c r="T54" s="8"/>
-      <c r="U54" s="8"/>
-      <c r="V54" s="8"/>
+      <c r="T54" s="8" t="n">
+        <v>0.167597198335865</v>
+      </c>
+      <c r="U54" s="8" t="n">
+        <v>0.171332844765486</v>
+      </c>
+      <c r="V54" s="8" t="n">
+        <v>0.174601042936443</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -2717,9 +2983,15 @@
       <c r="S55" s="8" t="n">
         <v>0.168930987356168</v>
       </c>
-      <c r="T55" s="8"/>
-      <c r="U55" s="8"/>
-      <c r="V55" s="8"/>
+      <c r="T55" s="8" t="n">
+        <v>0.171471853751967</v>
+      </c>
+      <c r="U55" s="8" t="n">
+        <v>0.174433661079199</v>
+      </c>
+      <c r="V55" s="8" t="n">
+        <v>0.178486052383916</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -2767,9 +3039,15 @@
       <c r="S56" s="8" t="n">
         <v>0.168676308401356</v>
       </c>
-      <c r="T56" s="8"/>
-      <c r="U56" s="8"/>
-      <c r="V56" s="8"/>
+      <c r="T56" s="8" t="n">
+        <v>0.173052654688399</v>
+      </c>
+      <c r="U56" s="8" t="n">
+        <v>0.176816967908337</v>
+      </c>
+      <c r="V56" s="8" t="n">
+        <v>0.180805610479004</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -2817,9 +3095,15 @@
       <c r="S57" s="8" t="n">
         <v>0.174695960335137</v>
       </c>
-      <c r="T57" s="8"/>
-      <c r="U57" s="8"/>
-      <c r="V57" s="8"/>
+      <c r="T57" s="8" t="n">
+        <v>0.177791873922312</v>
+      </c>
+      <c r="U57" s="8" t="n">
+        <v>0.181597139094902</v>
+      </c>
+      <c r="V57" s="8" t="n">
+        <v>0.186037417937448</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -2867,9 +3151,15 @@
       <c r="S58" s="8" t="n">
         <v>0.181444562174254</v>
       </c>
-      <c r="T58" s="8"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="8"/>
+      <c r="T58" s="8" t="n">
+        <v>0.185135261524696</v>
+      </c>
+      <c r="U58" s="8" t="n">
+        <v>0.188327828467154</v>
+      </c>
+      <c r="V58" s="8" t="n">
+        <v>0.193191823949389</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -2917,9 +3207,15 @@
       <c r="S59" s="8" t="n">
         <v>0.187295386017967</v>
       </c>
-      <c r="T59" s="8"/>
-      <c r="U59" s="8"/>
-      <c r="V59" s="8"/>
+      <c r="T59" s="8" t="n">
+        <v>0.191380780112426</v>
+      </c>
+      <c r="U59" s="8" t="n">
+        <v>0.195537980756271</v>
+      </c>
+      <c r="V59" s="8" t="n">
+        <v>0.200396776881478</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -2967,9 +3263,15 @@
       <c r="S60" s="8" t="n">
         <v>0.190661877248146</v>
       </c>
-      <c r="T60" s="8"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="8"/>
+      <c r="T60" s="8" t="n">
+        <v>0.197313931663039</v>
+      </c>
+      <c r="U60" s="8" t="n">
+        <v>0.201771867442493</v>
+      </c>
+      <c r="V60" s="8" t="n">
+        <v>0.206631731250354</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -3017,9 +3319,15 @@
       <c r="S61" s="8" t="n">
         <v>0.197867325085204</v>
       </c>
-      <c r="T61" s="8"/>
-      <c r="U61" s="8"/>
-      <c r="V61" s="8"/>
+      <c r="T61" s="8" t="n">
+        <v>0.201961441068795</v>
+      </c>
+      <c r="U61" s="8" t="n">
+        <v>0.206467624544912</v>
+      </c>
+      <c r="V61" s="8" t="n">
+        <v>0.212100197478496</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -3067,9 +3375,15 @@
       <c r="S62" s="8" t="n">
         <v>0.200744296433752</v>
       </c>
-      <c r="T62" s="8"/>
-      <c r="U62" s="8"/>
-      <c r="V62" s="8"/>
+      <c r="T62" s="8" t="n">
+        <v>0.205100850580019</v>
+      </c>
+      <c r="U62" s="8" t="n">
+        <v>0.208849747199537</v>
+      </c>
+      <c r="V62" s="8" t="n">
+        <v>0.215176586330566</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -3117,9 +3431,15 @@
       <c r="S63" s="8" t="n">
         <v>0.202169683703366</v>
       </c>
-      <c r="T63" s="8"/>
-      <c r="U63" s="8"/>
-      <c r="V63" s="8"/>
+      <c r="T63" s="8" t="n">
+        <v>0.20516378637029</v>
+      </c>
+      <c r="U63" s="8" t="n">
+        <v>0.210418530344818</v>
+      </c>
+      <c r="V63" s="8" t="n">
+        <v>0.216735273765241</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -3167,9 +3487,15 @@
       <c r="S64" s="8" t="n">
         <v>0.200806669778084</v>
       </c>
-      <c r="T64" s="8"/>
-      <c r="U64" s="8"/>
-      <c r="V64" s="8"/>
+      <c r="T64" s="8" t="n">
+        <v>0.203684049862136</v>
+      </c>
+      <c r="U64" s="8" t="n">
+        <v>0.209512873818142</v>
+      </c>
+      <c r="V64" s="8" t="n">
+        <v>0.215954230702011</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -3217,9 +3543,15 @@
       <c r="S65" s="8" t="n">
         <v>0.197315610088285</v>
       </c>
-      <c r="T65" s="8"/>
-      <c r="U65" s="8"/>
-      <c r="V65" s="8"/>
+      <c r="T65" s="8" t="n">
+        <v>0.201898267530631</v>
+      </c>
+      <c r="U65" s="8" t="n">
+        <v>0.207990122659556</v>
+      </c>
+      <c r="V65" s="8" t="n">
+        <v>0.215128101037872</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -3267,9 +3599,15 @@
       <c r="S66" s="8" t="n">
         <v>0.193508058641756</v>
       </c>
-      <c r="T66" s="8"/>
-      <c r="U66" s="8"/>
-      <c r="V66" s="8"/>
+      <c r="T66" s="8" t="n">
+        <v>0.198876871870007</v>
+      </c>
+      <c r="U66" s="8" t="n">
+        <v>0.20635573977322</v>
+      </c>
+      <c r="V66" s="8" t="n">
+        <v>0.214358306303063</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -3317,9 +3655,15 @@
       <c r="S67" s="8" t="n">
         <v>0.190664547845022</v>
       </c>
-      <c r="T67" s="8"/>
-      <c r="U67" s="8"/>
-      <c r="V67" s="8"/>
+      <c r="T67" s="8" t="n">
+        <v>0.195599529856785</v>
+      </c>
+      <c r="U67" s="8" t="n">
+        <v>0.204766278960429</v>
+      </c>
+      <c r="V67" s="8" t="n">
+        <v>0.214325863625456</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -3367,9 +3711,15 @@
       <c r="S68" s="8" t="n">
         <v>0.183088741789439</v>
       </c>
-      <c r="T68" s="8"/>
-      <c r="U68" s="8"/>
-      <c r="V68" s="8"/>
+      <c r="T68" s="8" t="n">
+        <v>0.1926467035612</v>
+      </c>
+      <c r="U68" s="8" t="n">
+        <v>0.202418966812647</v>
+      </c>
+      <c r="V68" s="8" t="n">
+        <v>0.213510004970129</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -3417,9 +3767,15 @@
       <c r="S69" s="8" t="n">
         <v>0.178312827007274</v>
       </c>
-      <c r="T69" s="8"/>
-      <c r="U69" s="8"/>
-      <c r="V69" s="8"/>
+      <c r="T69" s="8" t="n">
+        <v>0.188747901544975</v>
+      </c>
+      <c r="U69" s="8" t="n">
+        <v>0.20078195994845</v>
+      </c>
+      <c r="V69" s="8" t="n">
+        <v>0.211944640383383</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -3467,9 +3823,15 @@
       <c r="S70" s="8" t="n">
         <v>0.172019845644173</v>
       </c>
-      <c r="T70" s="8"/>
-      <c r="U70" s="8"/>
-      <c r="V70" s="8"/>
+      <c r="T70" s="8" t="n">
+        <v>0.184782911809714</v>
+      </c>
+      <c r="U70" s="8" t="n">
+        <v>0.197141004785713</v>
+      </c>
+      <c r="V70" s="8" t="n">
+        <v>0.209604286497979</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -3517,9 +3879,15 @@
       <c r="S71" s="8" t="n">
         <v>0.164221111235425</v>
       </c>
-      <c r="T71" s="8"/>
-      <c r="U71" s="8"/>
-      <c r="V71" s="8"/>
+      <c r="T71" s="8" t="n">
+        <v>0.178823936002527</v>
+      </c>
+      <c r="U71" s="8" t="n">
+        <v>0.192312814955329</v>
+      </c>
+      <c r="V71" s="8" t="n">
+        <v>0.205930747696473</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>